<commit_message>
Many changes. Working on getting database functionality for parameter lists
</commit_message>
<xml_diff>
--- a/V1000_Drive_Programmer/data/MACH_DATA.xlsx
+++ b/V1000_Drive_Programmer/data/MACH_DATA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="0" windowWidth="28800" windowHeight="12915"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="28800" windowHeight="12915"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>IDX</t>
   </si>
@@ -59,9 +59,6 @@
     <t>MLA</t>
   </si>
   <si>
-    <t>MOC</t>
-  </si>
-  <si>
     <t>MT2510</t>
   </si>
   <si>
@@ -101,21 +98,12 @@
     <t>L-A</t>
   </si>
   <si>
-    <t>MOC45</t>
-  </si>
-  <si>
-    <t>OC</t>
-  </si>
-  <si>
     <t>VSC</t>
   </si>
   <si>
     <t>M6</t>
   </si>
   <si>
-    <t>OC-45</t>
-  </si>
-  <si>
     <t>Translicer 2510</t>
   </si>
   <si>
@@ -125,37 +113,61 @@
     <t>Diversacut Sprint 2</t>
   </si>
   <si>
-    <t>VFD_CNT</t>
-  </si>
-  <si>
-    <t>VFD1_NAME</t>
-  </si>
-  <si>
-    <t>VFD2_NAME</t>
-  </si>
-  <si>
-    <t>Feed Motor</t>
-  </si>
-  <si>
-    <t>Drive Motor</t>
-  </si>
-  <si>
-    <t>Wheel Motor</t>
-  </si>
-  <si>
-    <t>Belt Motor</t>
-  </si>
-  <si>
-    <t>Feed &amp; Belt Motor</t>
-  </si>
-  <si>
-    <t>Primary Belt Motor</t>
-  </si>
-  <si>
-    <t>Secondary Belt Motor</t>
-  </si>
-  <si>
-    <t>VFD3_NAME</t>
+    <t>MOC/MOC45</t>
+  </si>
+  <si>
+    <t>OC/OC-45</t>
+  </si>
+  <si>
+    <t>DRV_CNT</t>
+  </si>
+  <si>
+    <t>DRV1_NAME</t>
+  </si>
+  <si>
+    <t>DRV2_NAME</t>
+  </si>
+  <si>
+    <t>DRV3_NAME</t>
+  </si>
+  <si>
+    <t>DRV4_NAME</t>
+  </si>
+  <si>
+    <t>DRV5_NAME</t>
+  </si>
+  <si>
+    <t>CHRT_CNT</t>
+  </si>
+  <si>
+    <t>CHRT1_PARTNUM</t>
+  </si>
+  <si>
+    <t>CHRT2_PARTNUM</t>
+  </si>
+  <si>
+    <t>CHRT3_PARTNUM</t>
+  </si>
+  <si>
+    <t>CHRT4_PARTNUM</t>
+  </si>
+  <si>
+    <t>CHRT5_PARTNUM</t>
+  </si>
+  <si>
+    <t>CHRT6_PARTNUM</t>
+  </si>
+  <si>
+    <t>CHRT7_PARTNUM</t>
+  </si>
+  <si>
+    <t>CHRT8_PARTNUM</t>
+  </si>
+  <si>
+    <t>CHRT9_PARTNUM</t>
+  </si>
+  <si>
+    <t>CHRT10_PARTNUM</t>
   </si>
 </sst>
 </file>
@@ -471,22 +483,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" customWidth="1"/>
     <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="20" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row spans="1:20" x14ac:dyDescent="0.2" outlineLevel="0" r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,19 +509,58 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
         <v>33</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="Q1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row spans="1:20" x14ac:dyDescent="0.2" outlineLevel="0" r="2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -517,16 +568,16 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row spans="1:20" x14ac:dyDescent="0.2" outlineLevel="0" r="3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -534,16 +585,16 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row spans="1:20" x14ac:dyDescent="0.2" outlineLevel="0" r="4">
       <c r="A4">
         <v>2</v>
       </c>
@@ -551,16 +602,16 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row spans="1:20" x14ac:dyDescent="0.2" outlineLevel="0" r="5">
       <c r="A5">
         <v>3</v>
       </c>
@@ -568,16 +619,16 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row spans="1:20" x14ac:dyDescent="0.2" outlineLevel="0" r="6">
       <c r="A6">
         <v>4</v>
       </c>
@@ -585,16 +636,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row spans="1:20" x14ac:dyDescent="0.2" outlineLevel="0" r="7">
       <c r="A7">
         <v>5</v>
       </c>
@@ -602,16 +653,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row spans="1:20" x14ac:dyDescent="0.2" outlineLevel="0" r="8">
       <c r="A8">
         <v>6</v>
       </c>
@@ -619,19 +670,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row spans="1:20" x14ac:dyDescent="0.2" outlineLevel="0" r="9">
       <c r="A9">
         <v>8</v>
       </c>
@@ -639,84 +687,84 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row spans="1:20" x14ac:dyDescent="0.2" outlineLevel="0" r="10">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row spans="1:20" x14ac:dyDescent="0.2" outlineLevel="0" r="11">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row spans="1:20" x14ac:dyDescent="0.2" outlineLevel="0" r="12">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row spans="1:20" x14ac:dyDescent="0.2" outlineLevel="0" r="13">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+    </row>
+    <row spans="1:20" x14ac:dyDescent="0.2" outlineLevel="0" r="14">
       <c r="A14">
         <v>13</v>
       </c>
@@ -724,56 +772,30 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row spans="1:20" x14ac:dyDescent="0.2" outlineLevel="0" r="15">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>39</v>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Various bug fixes: - Fixed issue with dB_Delete function not having the file extension for the spreadsheet. This was due to changing the function to work off of the database name rather than the full file name. - Changed how the VFD comm buttons work. It is now assumed communication is present and a drive is available as long as the comm port is detected rather than waiting for a read of the drive to enable communication to program parameters -  After programming the parameters in the scheduled change datagridview the clearing of the parameters also clears highlighted parameters in the full parameter view datagridview. - Added ability to remove a scheduled parameter change. Comes in handy when saving a modified parameter list and reloading it and having parameters that you don't want stored. - Added message box display to show parameters were successfully stored or deleted.
</commit_message>
<xml_diff>
--- a/V1000_Drive_Programmer/data/MACH_DATA.xlsx
+++ b/V1000_Drive_Programmer/data/MACH_DATA.xlsx
@@ -1,24 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sferry\source\repos\V1000_Drive_Programmer\V1000_Drive_Programmer\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="15120" yWindow="0" windowWidth="28800" windowHeight="12915"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" r:id="rId1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" fullCalcOnLoad="true"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}"/>
   </extLst>
 </workbook>
 </file>
@@ -538,7 +531,7 @@
         <v>38</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row spans="1:10" x14ac:dyDescent="0.2" outlineLevel="0" r="3">
@@ -661,7 +654,7 @@
         <v>41</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row spans="1:10" x14ac:dyDescent="0.2" outlineLevel="0" r="9">
@@ -790,7 +783,7 @@
         <v>41</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row spans="1:10" x14ac:dyDescent="0.2" outlineLevel="0" r="15">

</xml_diff>